<commit_message>
dashboard IPM Full Nasional + Sumbar clear
</commit_message>
<xml_diff>
--- a/IPM Nasional.xlsx
+++ b/IPM Nasional.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eja\nerwilis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68231C09-72C0-4692-BCA1-A7175B28EE55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B11391E0-2CCE-4AFC-B42E-D1B3CD1449CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Provinsi" sheetId="2" r:id="rId2"/>
     <sheet name="Pembagian" sheetId="3" r:id="rId3"/>
+    <sheet name="IDN Barat" sheetId="4" r:id="rId4"/>
+    <sheet name="IDN Tengah" sheetId="5" r:id="rId5"/>
+    <sheet name="IDN Timur" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2798" uniqueCount="1860">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2850" uniqueCount="1860">
   <si>
     <t>Provinsi/Kabupaten/Kota</t>
   </si>
@@ -15340,8 +15343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:J4"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A35" activeCellId="14" sqref="A21:XFD21 A22:XFD22 A23:XFD23 A24:XFD24 A25:XFD25 A26:XFD26 A27:XFD27 A28:XFD28 A29:XFD29 A30:XFD30 A31:XFD31 A32:XFD32 A33:XFD33 A34:XFD34 A35:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -15390,22 +15393,10 @@
         <f>AVERAGE(B2:E2)</f>
         <v>71.814999999999998</v>
       </c>
-      <c r="G2" s="1">
-        <f>AVERAGE(B2,B3,B4,B5,B6,B7,B8,B9,B10,B11,B12,B13,B17)</f>
-        <v>71.959230769230771</v>
-      </c>
-      <c r="H2" s="1">
-        <f t="shared" ref="H2:J2" si="0">AVERAGE(C2,C3,C4,C5,C6,C7,C8,C9,C10,C11,C12,C13,C17)</f>
-        <v>72.546153846153842</v>
-      </c>
-      <c r="I2" s="1">
-        <f t="shared" si="0"/>
-        <v>72.585384615384626</v>
-      </c>
-      <c r="J2" s="1">
-        <f t="shared" si="0"/>
-        <v>72.841538461538462</v>
-      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -15424,25 +15415,13 @@
         <v>72</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F36" si="1">AVERAGE(B3:E3)</f>
+        <f t="shared" ref="F3:F35" si="0">AVERAGE(B3:E3)</f>
         <v>71.672499999999999</v>
       </c>
-      <c r="G3" s="1">
-        <f>AVERAGE(B14,B15,B16,B18,B19,B20)</f>
-        <v>71.313333333333333</v>
-      </c>
-      <c r="H3" s="1">
-        <f t="shared" ref="H3:J3" si="2">AVERAGE(C14,C15,C16,C18,C19,C20)</f>
-        <v>71.995000000000005</v>
-      </c>
-      <c r="I3" s="1">
-        <f t="shared" si="2"/>
-        <v>72.081666666666663</v>
-      </c>
-      <c r="J3" s="1">
-        <f t="shared" si="2"/>
-        <v>72.356666666666669</v>
-      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -15461,25 +15440,13 @@
         <v>72.650000000000006</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>72.287499999999994</v>
       </c>
-      <c r="G4" s="1">
-        <f>AVERAGE(B21,B22,B23,B24,B25,B26,B27,B28,B29,B30,B31,B32,B33,B34,B35)</f>
-        <v>68.652666666666661</v>
-      </c>
-      <c r="H4" s="1">
-        <f t="shared" ref="H4:J4" si="3">AVERAGE(C21,C22,C23,C24,C25,C26,C27,C28,C29,C30,C31,C32,C33,C34,C35)</f>
-        <v>69.353333333333339</v>
-      </c>
-      <c r="I4" s="1">
-        <f t="shared" si="3"/>
-        <v>69.376666666666679</v>
-      </c>
-      <c r="J4" s="1">
-        <f t="shared" si="3"/>
-        <v>69.680000000000007</v>
-      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -15498,7 +15465,7 @@
         <v>72.94</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>72.772499999999994</v>
       </c>
     </row>
@@ -15519,7 +15486,7 @@
         <v>71.63</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>71.20750000000001</v>
       </c>
     </row>
@@ -15540,7 +15507,7 @@
         <v>70.239999999999995</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>69.915000000000006</v>
       </c>
     </row>
@@ -15561,7 +15528,7 @@
         <v>71.64</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>71.222499999999997</v>
       </c>
     </row>
@@ -15582,7 +15549,7 @@
         <v>69.900000000000006</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>69.544999999999987</v>
       </c>
     </row>
@@ -15603,7 +15570,7 @@
         <v>71.69</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>71.282499999999999</v>
       </c>
     </row>
@@ -15624,7 +15591,7 @@
         <v>75.790000000000006</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>75.424999999999997</v>
       </c>
     </row>
@@ -15645,7 +15612,7 @@
         <v>81.11</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>80.777500000000003</v>
       </c>
     </row>
@@ -15666,7 +15633,7 @@
         <v>72.45</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>71.967500000000001</v>
       </c>
     </row>
@@ -15687,7 +15654,7 @@
         <v>72.16</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>71.72</v>
       </c>
     </row>
@@ -15708,7 +15675,7 @@
         <v>80.22</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>79.927499999999995</v>
       </c>
     </row>
@@ -15729,7 +15696,7 @@
         <v>72.14</v>
       </c>
       <c r="F16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>71.529999999999987</v>
       </c>
     </row>
@@ -15750,7 +15717,7 @@
         <v>72.72</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>72.389999999999986</v>
       </c>
     </row>
@@ -15771,7 +15738,7 @@
         <v>75.69</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>75.334999999999994</v>
       </c>
     </row>
@@ -15792,7 +15759,7 @@
         <v>68.650000000000006</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>68.085000000000008</v>
       </c>
     </row>
@@ -15813,7 +15780,7 @@
         <v>65.28</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>65.022500000000008</v>
       </c>
     </row>
@@ -15834,7 +15801,7 @@
         <v>67.900000000000006</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>67.547499999999999</v>
       </c>
     </row>
@@ -15855,7 +15822,7 @@
         <v>71.25</v>
       </c>
       <c r="F22" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>70.907499999999999</v>
       </c>
     </row>
@@ -15876,7 +15843,7 @@
         <v>71.28</v>
       </c>
       <c r="F23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>70.77</v>
       </c>
     </row>
@@ -15897,7 +15864,7 @@
         <v>76.88</v>
       </c>
       <c r="F24" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>76.39</v>
       </c>
     </row>
@@ -15918,7 +15885,7 @@
         <v>71.19</v>
       </c>
       <c r="F25" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>70.882499999999993</v>
       </c>
     </row>
@@ -15939,7 +15906,7 @@
         <v>73.3</v>
       </c>
       <c r="F26" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>72.855000000000004</v>
       </c>
     </row>
@@ -15960,7 +15927,7 @@
         <v>69.790000000000006</v>
       </c>
       <c r="F27" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>69.430000000000007</v>
       </c>
     </row>
@@ -15981,7 +15948,7 @@
         <v>72.239999999999995</v>
       </c>
       <c r="F28" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>71.682500000000005</v>
       </c>
     </row>
@@ -16002,7 +15969,7 @@
         <v>71.66</v>
       </c>
       <c r="F29" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>71.22999999999999</v>
       </c>
     </row>
@@ -16023,7 +15990,7 @@
         <v>69</v>
       </c>
       <c r="F30" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>68.47</v>
       </c>
     </row>
@@ -16044,7 +16011,7 @@
         <v>66.36</v>
       </c>
       <c r="F31" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>65.825000000000003</v>
       </c>
     </row>
@@ -16065,7 +16032,7 @@
         <v>69.709999999999994</v>
       </c>
       <c r="F32" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>69.38</v>
       </c>
     </row>
@@ -16086,7 +16053,7 @@
         <v>68.760000000000005</v>
       </c>
       <c r="F33" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>68.427499999999995</v>
       </c>
     </row>
@@ -16107,7 +16074,7 @@
         <v>65.260000000000005</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>64.697500000000005</v>
       </c>
     </row>
@@ -16128,7 +16095,7 @@
         <v>60.62</v>
       </c>
       <c r="F35" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>60.49</v>
       </c>
     </row>
@@ -16149,7 +16116,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED9A115-3AAD-40F1-AEB0-1EC85D95E7C4}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -16226,4 +16193,804 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62FAB9B9-F3ED-44C9-B458-61C5E36226F1}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1850</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1851</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1852</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1853</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1854</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1855</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1">
+        <v>71.19</v>
+      </c>
+      <c r="C2" s="1">
+        <v>71.900000000000006</v>
+      </c>
+      <c r="D2" s="1">
+        <v>71.989999999999995</v>
+      </c>
+      <c r="E2" s="1">
+        <v>72.180000000000007</v>
+      </c>
+      <c r="F2" s="1">
+        <v>71.814999999999998</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" s="1">
+        <v>71.180000000000007</v>
+      </c>
+      <c r="C3" s="1">
+        <v>71.739999999999995</v>
+      </c>
+      <c r="D3" s="1">
+        <v>71.77</v>
+      </c>
+      <c r="E3" s="1">
+        <v>72</v>
+      </c>
+      <c r="F3" s="1">
+        <v>71.672499999999999</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>281</v>
+      </c>
+      <c r="B4" s="1">
+        <v>71.73</v>
+      </c>
+      <c r="C4" s="1">
+        <v>72.39</v>
+      </c>
+      <c r="D4" s="1">
+        <v>72.38</v>
+      </c>
+      <c r="E4" s="1">
+        <v>72.650000000000006</v>
+      </c>
+      <c r="F4" s="1">
+        <v>72.287499999999994</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>368</v>
+      </c>
+      <c r="B5" s="1">
+        <v>72.44</v>
+      </c>
+      <c r="C5" s="1">
+        <v>73</v>
+      </c>
+      <c r="D5" s="1">
+        <v>72.709999999999994</v>
+      </c>
+      <c r="E5" s="1">
+        <v>72.94</v>
+      </c>
+      <c r="F5" s="1">
+        <v>72.772499999999994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>425</v>
+      </c>
+      <c r="B6" s="1">
+        <v>70.650000000000006</v>
+      </c>
+      <c r="C6" s="1">
+        <v>71.260000000000005</v>
+      </c>
+      <c r="D6" s="1">
+        <v>71.290000000000006</v>
+      </c>
+      <c r="E6" s="1">
+        <v>71.63</v>
+      </c>
+      <c r="F6" s="1">
+        <v>71.20750000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>472</v>
+      </c>
+      <c r="B7" s="1">
+        <v>69.39</v>
+      </c>
+      <c r="C7" s="1">
+        <v>70.02</v>
+      </c>
+      <c r="D7" s="1">
+        <v>70.010000000000005</v>
+      </c>
+      <c r="E7" s="1">
+        <v>70.239999999999995</v>
+      </c>
+      <c r="F7" s="1">
+        <v>69.915000000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>542</v>
+      </c>
+      <c r="B8" s="1">
+        <v>70.64</v>
+      </c>
+      <c r="C8" s="1">
+        <v>71.209999999999994</v>
+      </c>
+      <c r="D8" s="1">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="E8" s="1">
+        <v>71.64</v>
+      </c>
+      <c r="F8" s="1">
+        <v>71.222499999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>580</v>
+      </c>
+      <c r="B9" s="1">
+        <v>69.02</v>
+      </c>
+      <c r="C9" s="1">
+        <v>69.569999999999993</v>
+      </c>
+      <c r="D9" s="1">
+        <v>69.69</v>
+      </c>
+      <c r="E9" s="1">
+        <v>69.900000000000006</v>
+      </c>
+      <c r="F9" s="1">
+        <v>69.544999999999987</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>636</v>
+      </c>
+      <c r="B10" s="1">
+        <v>70.67</v>
+      </c>
+      <c r="C10" s="1">
+        <v>71.3</v>
+      </c>
+      <c r="D10" s="1">
+        <v>71.47</v>
+      </c>
+      <c r="E10" s="1">
+        <v>71.69</v>
+      </c>
+      <c r="F10" s="1">
+        <v>71.282499999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>658</v>
+      </c>
+      <c r="B11" s="1">
+        <v>74.84</v>
+      </c>
+      <c r="C11" s="1">
+        <v>75.48</v>
+      </c>
+      <c r="D11" s="1">
+        <v>75.59</v>
+      </c>
+      <c r="E11" s="1">
+        <v>75.790000000000006</v>
+      </c>
+      <c r="F11" s="1">
+        <v>75.424999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>687</v>
+      </c>
+      <c r="B12" s="1">
+        <v>80.47</v>
+      </c>
+      <c r="C12" s="1">
+        <v>80.760000000000005</v>
+      </c>
+      <c r="D12" s="1">
+        <v>80.77</v>
+      </c>
+      <c r="E12" s="1">
+        <v>81.11</v>
+      </c>
+      <c r="F12" s="1">
+        <v>80.777500000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>717</v>
+      </c>
+      <c r="B13" s="1">
+        <v>71.3</v>
+      </c>
+      <c r="C13" s="1">
+        <v>72.03</v>
+      </c>
+      <c r="D13" s="1">
+        <v>72.09</v>
+      </c>
+      <c r="E13" s="1">
+        <v>72.45</v>
+      </c>
+      <c r="F13" s="1">
+        <v>71.967500000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B14" s="1">
+        <v>71.95</v>
+      </c>
+      <c r="C14" s="1">
+        <v>72.44</v>
+      </c>
+      <c r="D14" s="1">
+        <v>72.45</v>
+      </c>
+      <c r="E14" s="1">
+        <v>72.72</v>
+      </c>
+      <c r="F14" s="1">
+        <v>72.389999999999986</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E601271-B689-4102-8BB2-CC9B811FB7D1}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1850</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1851</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1852</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1853</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1854</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1855</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>818</v>
+      </c>
+      <c r="B2" s="1">
+        <v>71.12</v>
+      </c>
+      <c r="C2" s="1">
+        <v>71.73</v>
+      </c>
+      <c r="D2" s="1">
+        <v>71.87</v>
+      </c>
+      <c r="E2" s="1">
+        <v>72.16</v>
+      </c>
+      <c r="F2" s="1">
+        <v>71.72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>937</v>
+      </c>
+      <c r="B3" s="1">
+        <v>79.53</v>
+      </c>
+      <c r="C3" s="1">
+        <v>79.989999999999995</v>
+      </c>
+      <c r="D3" s="1">
+        <v>79.97</v>
+      </c>
+      <c r="E3" s="1">
+        <v>80.22</v>
+      </c>
+      <c r="F3" s="1">
+        <v>79.927499999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>960</v>
+      </c>
+      <c r="B4" s="1">
+        <v>70.77</v>
+      </c>
+      <c r="C4" s="1">
+        <v>71.5</v>
+      </c>
+      <c r="D4" s="1">
+        <v>71.709999999999994</v>
+      </c>
+      <c r="E4" s="1">
+        <v>72.14</v>
+      </c>
+      <c r="F4" s="1">
+        <v>71.529999999999987</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B5" s="1">
+        <v>74.77</v>
+      </c>
+      <c r="C5" s="1">
+        <v>75.38</v>
+      </c>
+      <c r="D5" s="1">
+        <v>75.5</v>
+      </c>
+      <c r="E5" s="1">
+        <v>75.69</v>
+      </c>
+      <c r="F5" s="1">
+        <v>75.334999999999994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B6" s="1">
+        <v>67.3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>68.14</v>
+      </c>
+      <c r="D6" s="1">
+        <v>68.25</v>
+      </c>
+      <c r="E6" s="1">
+        <v>68.650000000000006</v>
+      </c>
+      <c r="F6" s="1">
+        <v>68.085000000000008</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1188</v>
+      </c>
+      <c r="B7" s="1">
+        <v>64.39</v>
+      </c>
+      <c r="C7" s="1">
+        <v>65.23</v>
+      </c>
+      <c r="D7" s="1">
+        <v>65.19</v>
+      </c>
+      <c r="E7" s="1">
+        <v>65.28</v>
+      </c>
+      <c r="F7" s="1">
+        <v>65.022500000000008</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F95D14-3FB1-49BF-A276-018ECDE2883E}">
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1850</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1851</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1852</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1853</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1854</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1855</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B2" s="1">
+        <v>66.98</v>
+      </c>
+      <c r="C2" s="1">
+        <v>67.650000000000006</v>
+      </c>
+      <c r="D2" s="1">
+        <v>67.66</v>
+      </c>
+      <c r="E2" s="1">
+        <v>67.900000000000006</v>
+      </c>
+      <c r="F2" s="1">
+        <v>67.547499999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1323</v>
+      </c>
+      <c r="B3" s="1">
+        <v>70.42</v>
+      </c>
+      <c r="C3" s="1">
+        <v>70.91</v>
+      </c>
+      <c r="D3" s="1">
+        <v>71.05</v>
+      </c>
+      <c r="E3" s="1">
+        <v>71.25</v>
+      </c>
+      <c r="F3" s="1">
+        <v>70.907499999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1352</v>
+      </c>
+      <c r="B4" s="1">
+        <v>70.17</v>
+      </c>
+      <c r="C4" s="1">
+        <v>70.72</v>
+      </c>
+      <c r="D4" s="1">
+        <v>70.91</v>
+      </c>
+      <c r="E4" s="1">
+        <v>71.28</v>
+      </c>
+      <c r="F4" s="1">
+        <v>70.77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1387</v>
+      </c>
+      <c r="B5" s="1">
+        <v>75.83</v>
+      </c>
+      <c r="C5" s="1">
+        <v>76.61</v>
+      </c>
+      <c r="D5" s="1">
+        <v>76.239999999999995</v>
+      </c>
+      <c r="E5" s="1">
+        <v>76.88</v>
+      </c>
+      <c r="F5" s="1">
+        <v>76.39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1421</v>
+      </c>
+      <c r="B6" s="1">
+        <v>70.56</v>
+      </c>
+      <c r="C6" s="1">
+        <v>71.150000000000006</v>
+      </c>
+      <c r="D6" s="1">
+        <v>70.63</v>
+      </c>
+      <c r="E6" s="1">
+        <v>71.19</v>
+      </c>
+      <c r="F6" s="1">
+        <v>70.882499999999993</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1434</v>
+      </c>
+      <c r="B7" s="1">
+        <v>72.2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>72.989999999999995</v>
+      </c>
+      <c r="D7" s="1">
+        <v>72.930000000000007</v>
+      </c>
+      <c r="E7" s="1">
+        <v>73.3</v>
+      </c>
+      <c r="F7" s="1">
+        <v>72.855000000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1471</v>
+      </c>
+      <c r="B8" s="1">
+        <v>68.88</v>
+      </c>
+      <c r="C8" s="1">
+        <v>69.5</v>
+      </c>
+      <c r="D8" s="1">
+        <v>69.55</v>
+      </c>
+      <c r="E8" s="1">
+        <v>69.790000000000006</v>
+      </c>
+      <c r="F8" s="1">
+        <v>69.430000000000007</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1504</v>
+      </c>
+      <c r="B9" s="1">
+        <v>70.900000000000006</v>
+      </c>
+      <c r="C9" s="1">
+        <v>71.66</v>
+      </c>
+      <c r="D9" s="1">
+        <v>71.930000000000007</v>
+      </c>
+      <c r="E9" s="1">
+        <v>72.239999999999995</v>
+      </c>
+      <c r="F9" s="1">
+        <v>71.682500000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1559</v>
+      </c>
+      <c r="B10" s="1">
+        <v>70.61</v>
+      </c>
+      <c r="C10" s="1">
+        <v>71.2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>71.45</v>
+      </c>
+      <c r="E10" s="1">
+        <v>71.66</v>
+      </c>
+      <c r="F10" s="1">
+        <v>71.22999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1596</v>
+      </c>
+      <c r="B11" s="1">
+        <v>67.709999999999994</v>
+      </c>
+      <c r="C11" s="1">
+        <v>68.489999999999995</v>
+      </c>
+      <c r="D11" s="1">
+        <v>68.680000000000007</v>
+      </c>
+      <c r="E11" s="1">
+        <v>69</v>
+      </c>
+      <c r="F11" s="1">
+        <v>68.47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1612</v>
+      </c>
+      <c r="B12" s="1">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="C12" s="1">
+        <v>65.73</v>
+      </c>
+      <c r="D12" s="1">
+        <v>66.11</v>
+      </c>
+      <c r="E12" s="1">
+        <v>66.36</v>
+      </c>
+      <c r="F12" s="1">
+        <v>65.825000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1630</v>
+      </c>
+      <c r="B13" s="1">
+        <v>68.87</v>
+      </c>
+      <c r="C13" s="1">
+        <v>69.45</v>
+      </c>
+      <c r="D13" s="1">
+        <v>69.489999999999995</v>
+      </c>
+      <c r="E13" s="1">
+        <v>69.709999999999994</v>
+      </c>
+      <c r="F13" s="1">
+        <v>69.38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1663</v>
+      </c>
+      <c r="B14" s="1">
+        <v>67.760000000000005</v>
+      </c>
+      <c r="C14" s="1">
+        <v>68.7</v>
+      </c>
+      <c r="D14" s="1">
+        <v>68.489999999999995</v>
+      </c>
+      <c r="E14" s="1">
+        <v>68.760000000000005</v>
+      </c>
+      <c r="F14" s="1">
+        <v>68.427499999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1691</v>
+      </c>
+      <c r="B15" s="1">
+        <v>63.74</v>
+      </c>
+      <c r="C15" s="1">
+        <v>64.7</v>
+      </c>
+      <c r="D15" s="1">
+        <v>65.09</v>
+      </c>
+      <c r="E15" s="1">
+        <v>65.260000000000005</v>
+      </c>
+      <c r="F15" s="1">
+        <v>64.697500000000005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1736</v>
+      </c>
+      <c r="B16" s="1">
+        <v>60.06</v>
+      </c>
+      <c r="C16" s="1">
+        <v>60.84</v>
+      </c>
+      <c r="D16" s="1">
+        <v>60.44</v>
+      </c>
+      <c r="E16" s="1">
+        <v>60.62</v>
+      </c>
+      <c r="F16" s="1">
+        <v>60.49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>